<commit_message>
Auto-synced Excel and Markdown tables
</commit_message>
<xml_diff>
--- a/tables/table_Campylobacter.xlsx
+++ b/tables/table_Campylobacter.xlsx
@@ -461,7 +461,11 @@
           <t>**国立医薬品食品衛生研究所** &lt;br&gt; 厚生労働科学研究費（食品の安全確保推進研究事業） &lt;br&gt; 「と畜・食鳥処理場におけるHACCP検証方法の確立と食鳥処理工程の高度衛生管理に関する研究」 &lt;br&gt; 分担研究報告書[「生食用食鳥肉の高度衛生管理に関する研究」](https://mhlw-grants.niph.go.jp/system/files/report_pdf/11.%20%E5%88%86%E6%8B%85%E7%A0%94%E7%A9%B6%E2%91%A5%20p77-97.pdf) &lt;br&gt; -　関連論文の[リンク](https://www.jstage.jst.go.jp/article/jvms/84/3/84_21-0486/_pdf/-char/ja)</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -491,7 +495,11 @@
           <t>**国立医薬品食品衛生研究所** &lt;br&gt; 食品健康影響評価技術研究 &lt;br&gt; [鶏肉のフードチェーンを通じたカンピロバクターの定量的動態解析とリスク低減効果の評価に向けた研究（鶏肉中のカンピロバクターのリスク評価手法に関する研究）](https://www.fsc.go.jp/fsciis/attachedFile/download?retrievalId=cho99920222202&amp;fileId=001)</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -521,7 +529,11 @@
           <t>**国立医薬品食品衛生研究所** &lt;br&gt; 厚生労働科学研究費（食品の安全確保推進研究事業）&lt;br&gt;「畜産食品の生物学的ハザードとそのリスクを低減するための研究」&lt;br&gt;分担研究報告書[「鶏肉食品におけるカンピロバクター等の定量的汚染実態に関する研究」](https://mhlw-grants.niph.go.jp/system/files/report_pdf/R3%E6%9C%9D%E5%80%89%E5%88%86%E6%8B%85%E7%A0%94%E7%A9%B6%E5%A0%B1%E5%91%8A%E6%9B%B8.doc__0.pdf)</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -568,7 +580,11 @@
           <t>**国立医薬品食品衛生研究所** &lt;br&gt; 厚生労働科学研究費（食品の安全確保推進研究事業）&lt;br&gt;「畜産食品の生物学的ハザードとそのリスクを低減するための研究」&lt;br&gt;分担研究報告書[「鶏肉食品におけるカンピロバクター等の定量的汚染実態に関する研究」](https://mhlw-grants.niph.go.jp/system/files/2019/193031/201924021A_upload/201924021A0004.pdf)</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr"/>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -598,7 +614,11 @@
           <t>**新潟県長岡食肉衛生検査センター** &lt;br&gt; [新潟県における市販鶏肉のカンピロバクター汚染調査](https://www.jstage.jst.go.jp/article/jvma/71/3/71_149/_pdf)</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -628,7 +648,11 @@
           <t>**国立医薬品食品衛生研究所** &lt;br&gt; 厚生労働科学研究費（食品の安全確保推進研究事業）&lt;br&gt; [と畜・食鳥検査における疾病診断の標準化とカンピロバクター等の制御に関する研究](https://mhlw-grants.niph.go.jp/project/24503)</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -658,7 +682,11 @@
           <t>**岐阜県食肉衛生検査所** &lt;br&gt; [牛胆嚢内胆汁のカンピロバクター汚染と胆汁の生化学的性状](https://warp.ndl.go.jp/info:ndljp/pid/11533510/www.pref.gifu.lg.jp/kurashi/shoku/shokuhin/22513/gakkai-tou-happyou.data/24-13.pdf)</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -671,7 +699,11 @@
           <t>**公益財団法人鹿児島市獣医公衆衛生協会** &lt;br&gt; [食鳥処理工程におけるカンピロバクター等微生物汚染防止低減への取り組みについて](https://warp.ndl.go.jp/info:ndljp/pid/12996857/www.jyuieisei-kgo.jp/topics/sozai/researchextract01_2011.pdf)</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -701,7 +733,11 @@
           <t>**埼玉県衛生研究所** &lt;br&gt; [市販鶏肉のカンピロバクター及びサルモネラ汚染状況と分離株の薬剤感受性](https://jvma-vet.jp/mag/06706/d2.pdf)</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr"/>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -714,7 +750,11 @@
           <t>**宮城県保健環境センター** &lt;br&gt; [市販食肉等からのカンピロバクター検出と低温保存での菌消長](https://www.pref.miyagi.jp/documents/1979/209066.pdf)</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -727,7 +767,11 @@
           <t>**埼玉県衛生研究所** &lt;br&gt; [MPN法および直接平板塗抹法による市販鶏レバーのカンピロバクターの定量検査](https://www.jstage.jst.go.jp/article/jvma1951/55/7/55_7_447/_pdf/-char/en)</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -740,7 +784,11 @@
           <t>**岩手大学** &lt;br&gt; 厚生労働科学研究費（特別研究事業） &lt;br&gt; [鶏肉に起因するカンピロバクター食中毒の予防対策に関する調査研究](https://warp.ndl.go.jp/collections/content/info:ndljp/pid/13046218/mhlw-grants.niph.go.jp/project/3941)</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -753,7 +801,11 @@
           <t>**埼玉県衛生研究所** &lt;br&gt; [市販鶏肉におけるカンピロバクターの定量検査と分離菌株の血清型](https://www.jstage.jst.go.jp/article/jvma1951/57/9/57_9_595/_pdf/-char/ja)</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -766,7 +818,11 @@
           <t>**埼玉県衛生研究所** &lt;br&gt; [国産および輸入鶏肉におけるカンピロバクターの汚染状況](https://agriknowledge.affrc.go.jp/RN/2010671140.pdf)</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Synced Excel tables from Markdown
</commit_message>
<xml_diff>
--- a/tables/table_Campylobacter.xlsx
+++ b/tables/table_Campylobacter.xlsx
@@ -730,12 +730,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>**埼玉県衛生研究所** &lt;br&gt; [市販鶏肉のカンピロバクター及びサルモネラ汚染状況と分離株の薬剤感受性](https://jvma-vet.jp/mag/06706/d2.pdf)</t>
+          <t>**埼玉県衛生研究所** &lt;br&gt; [市販鶏肉のカンピロバクター及びサルモネラ汚染状況と分離株の薬剤感受性](https://jvma-vet.jp/mag/06706/d2.pdf) &lt;br&gt;（日獣会誌, 67, 442~448, 2014）</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>未登録</t>
+          <t>済</t>
         </is>
       </c>
     </row>

</xml_diff>